<commit_message>
added support for creating and editing categories
</commit_message>
<xml_diff>
--- a/sheets/schedule.xlsx
+++ b/sheets/schedule.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achintya/blackboard/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C262FD-4973-0344-AD36-1A68541989AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317D0D25-DD89-4045-A81E-ADCA6A4FB644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31060" yWindow="3460" windowWidth="28040" windowHeight="17440" xr2:uid="{0380C0C1-920A-D840-98C9-90EA17E4F7E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="35">
   <si>
     <t>Tutorial</t>
   </si>
@@ -98,18 +98,6 @@
     <t>15:25</t>
   </si>
   <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
     <t>Homeroom</t>
   </si>
   <si>
@@ -144,6 +132,12 @@
   </si>
   <si>
     <t>09:30</t>
+  </si>
+  <si>
+    <t>08:40</t>
+  </si>
+  <si>
+    <t>09:25</t>
   </si>
 </sst>
 </file>
@@ -511,34 +505,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A42BE7A-AE95-1744-85F5-F7E71EBBCBEF}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -551,8 +545,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>21</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -565,8 +559,8 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -579,8 +573,8 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -593,8 +587,8 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>21</v>
+      <c r="B6">
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -607,8 +601,8 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
+      <c r="B7">
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -621,8 +615,8 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>21</v>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
@@ -635,8 +629,8 @@
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
+      <c r="B9">
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
@@ -649,8 +643,8 @@
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
+      <c r="B10">
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
@@ -663,8 +657,8 @@
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>21</v>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
@@ -677,39 +671,39 @@
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
-        <v>22</v>
+      <c r="B14">
+        <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -719,11 +713,11 @@
       <c r="A15">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
-        <v>22</v>
+      <c r="B15">
+        <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
@@ -733,8 +727,8 @@
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
-        <v>22</v>
+      <c r="B16">
+        <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>10</v>
@@ -747,36 +741,36 @@
       <c r="A17">
         <v>6</v>
       </c>
-      <c r="B17" t="s">
-        <v>22</v>
+      <c r="B17">
+        <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
-      <c r="B18" t="s">
-        <v>23</v>
+      <c r="B18">
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
-        <v>23</v>
+      <c r="B19">
+        <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
@@ -789,8 +783,8 @@
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
-        <v>23</v>
+      <c r="B20">
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
@@ -803,8 +797,8 @@
       <c r="A21">
         <v>3</v>
       </c>
-      <c r="B21" t="s">
-        <v>23</v>
+      <c r="B21">
+        <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>8</v>
@@ -817,8 +811,8 @@
       <c r="A22" t="s">
         <v>2</v>
       </c>
-      <c r="B22" t="s">
-        <v>23</v>
+      <c r="B22">
+        <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>10</v>
@@ -831,22 +825,22 @@
       <c r="A23">
         <v>7</v>
       </c>
-      <c r="B23" t="s">
-        <v>23</v>
+      <c r="B23">
+        <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
-      <c r="B24" t="s">
-        <v>24</v>
+      <c r="B24">
+        <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
@@ -859,8 +853,8 @@
       <c r="A25">
         <v>2</v>
       </c>
-      <c r="B25" t="s">
-        <v>24</v>
+      <c r="B25">
+        <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>4</v>
@@ -873,8 +867,8 @@
       <c r="A26" t="s">
         <v>0</v>
       </c>
-      <c r="B26" t="s">
-        <v>24</v>
+      <c r="B26">
+        <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
@@ -887,8 +881,8 @@
       <c r="A27">
         <v>3</v>
       </c>
-      <c r="B27" t="s">
-        <v>24</v>
+      <c r="B27">
+        <v>4</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
@@ -901,8 +895,8 @@
       <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B28" t="s">
-        <v>24</v>
+      <c r="B28">
+        <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>7</v>
@@ -915,8 +909,8 @@
       <c r="A29">
         <v>4</v>
       </c>
-      <c r="B29" t="s">
-        <v>24</v>
+      <c r="B29">
+        <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>8</v>
@@ -929,8 +923,8 @@
       <c r="A30">
         <v>5</v>
       </c>
-      <c r="B30" t="s">
-        <v>24</v>
+      <c r="B30">
+        <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>9</v>
@@ -943,8 +937,8 @@
       <c r="A31" t="s">
         <v>2</v>
       </c>
-      <c r="B31" t="s">
-        <v>24</v>
+      <c r="B31">
+        <v>4</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>10</v>
@@ -957,8 +951,8 @@
       <c r="A32">
         <v>6</v>
       </c>
-      <c r="B32" t="s">
-        <v>24</v>
+      <c r="B32">
+        <v>4</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>11</v>
@@ -971,13 +965,139 @@
       <c r="A33">
         <v>7</v>
       </c>
-      <c r="B33" t="s">
-        <v>24</v>
+      <c r="B33">
+        <v>4</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>